<commit_message>
updates from JAs end of summer report
</commit_message>
<xml_diff>
--- a/data/Kirby_NyackMC/nmc_meta.xlsx
+++ b/data/Kirby_NyackMC/nmc_meta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Dropbox\Kirby_priming\DOC_priming\data\Kirby_NyackMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{653CBB19-70BF-404A-8F3B-35A281EB736A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF6634CC-4CB2-4FAA-8EE9-DDBD3C8504E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A69F203D-439C-47CC-869C-6C2FECF3AFA4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="48">
   <si>
     <t>Syringe</t>
   </si>
@@ -78,6 +78,108 @@
   </si>
   <si>
     <t>BH13</t>
+  </si>
+  <si>
+    <t>NI1</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>NI110</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>NI2</t>
+  </si>
+  <si>
+    <t>NI89</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>NI16</t>
+  </si>
+  <si>
+    <t>NI19</t>
+  </si>
+  <si>
+    <t>NI139</t>
+  </si>
+  <si>
+    <t>NI10</t>
+  </si>
+  <si>
+    <t>NI98</t>
+  </si>
+  <si>
+    <t>NI118</t>
+  </si>
+  <si>
+    <t>NI22</t>
+  </si>
+  <si>
+    <t>NI3</t>
+  </si>
+  <si>
+    <t>NI84</t>
+  </si>
+  <si>
+    <t>NI114</t>
+  </si>
+  <si>
+    <t>NI119</t>
+  </si>
+  <si>
+    <t>NI123</t>
+  </si>
+  <si>
+    <t>NI138</t>
+  </si>
+  <si>
+    <t>NI103</t>
+  </si>
+  <si>
+    <t>NI5</t>
+  </si>
+  <si>
+    <t>NI105</t>
+  </si>
+  <si>
+    <t>NI69</t>
+  </si>
+  <si>
+    <t>U033</t>
+  </si>
+  <si>
+    <t>BH16</t>
+  </si>
+  <si>
+    <t>U030</t>
+  </si>
+  <si>
+    <t>U005</t>
+  </si>
+  <si>
+    <t>U048</t>
+  </si>
+  <si>
+    <t>BH05</t>
+  </si>
+  <si>
+    <t>U018</t>
+  </si>
+  <si>
+    <t>BH20</t>
+  </si>
+  <si>
+    <t>replicate</t>
+  </si>
+  <si>
+    <t>014</t>
   </si>
 </sst>
 </file>
@@ -113,10 +215,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD47986-9BB1-4DA9-A9D3-6DC933AAC2F5}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -444,7 +547,7 @@
     <col min="6" max="6" width="12.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,8 +566,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -481,11 +587,11 @@
         <v>0.50763888888888886</v>
       </c>
       <c r="F2">
-        <f>26.92/760</f>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <f t="shared" ref="F2:F11" si="0">26.92*0.033421</f>
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>81</v>
       </c>
@@ -502,11 +608,11 @@
         <v>0.50763888888888886</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F17" si="0">26.92/760</f>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="0"/>
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -524,10 +630,10 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -545,10 +651,10 @@
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -566,10 +672,10 @@
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -587,10 +693,10 @@
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -608,10 +714,10 @@
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -629,10 +735,10 @@
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>55</v>
       </c>
@@ -650,10 +756,10 @@
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>37</v>
       </c>
@@ -671,10 +777,10 @@
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -691,11 +797,11 @@
         <v>0.54236111111111118</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <f>26.92*0.033421</f>
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>95</v>
       </c>
@@ -712,11 +818,11 @@
         <v>0.54236111111111118</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+        <f t="shared" ref="F13:F17" si="1">26.92*0.033421</f>
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>33</v>
       </c>
@@ -733,11 +839,11 @@
         <v>0.55694444444444446</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>82</v>
       </c>
@@ -754,11 +860,11 @@
         <v>0.55694444444444446</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>5</v>
       </c>
@@ -775,11 +881,11 @@
         <v>0.56319444444444444</v>
       </c>
       <c r="F16">
-        <f t="shared" si="0"/>
-        <v>3.542105263157895E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <f t="shared" si="1"/>
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>79</v>
       </c>
@@ -796,8 +902,1160 @@
         <v>0.56319444444444444</v>
       </c>
       <c r="F17">
-        <f t="shared" si="0"/>
-        <v>3.542105263157895E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.89969332000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="F18">
+        <f>26.83*0.033421</f>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ref="F19:F65" si="2">26.83*0.033421</f>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.67083333333333339</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.67083333333333339</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.67152777777777783</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.67152777777777783</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.67638888888888893</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.67638888888888893</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.67847222222222225</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G28" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.67847222222222225</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.68472222222222223</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.68472222222222223</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G31" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.68611111111111101</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.68611111111111101</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.68611111111111101</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0.68611111111111101</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G35" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0.69236111111111109</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.69236111111111109</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0.69374999999999998</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G42" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>53</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G43" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0.7006944444444444</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46">
+        <v>5</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>6</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E48" s="2">
+        <v>0.70694444444444438</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G48" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>92</v>
+      </c>
+      <c r="B49">
+        <v>6</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0.70694444444444438</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50">
+        <v>6</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E50" s="2">
+        <v>0.70763888888888893</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G50" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>13</v>
+      </c>
+      <c r="B51">
+        <v>6</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0.70763888888888893</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G51" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>31</v>
+      </c>
+      <c r="B52">
+        <v>6</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>126</v>
+      </c>
+      <c r="B53">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E53" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>30</v>
+      </c>
+      <c r="B54">
+        <v>7</v>
+      </c>
+      <c r="C54">
+        <v>2</v>
+      </c>
+      <c r="D54" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E54" s="2">
+        <v>0.71319444444444446</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55">
+        <v>7</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E55" s="2">
+        <v>0.71319444444444446</v>
+      </c>
+      <c r="F55">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56">
+        <v>7</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0.71388888888888891</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>43</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0.71388888888888891</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G57" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <v>7</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0.71458333333333324</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G58" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>70</v>
+      </c>
+      <c r="B59">
+        <v>7</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0.71458333333333324</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G59" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60">
+        <v>8</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E60" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G60" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>82</v>
+      </c>
+      <c r="B61">
+        <v>8</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0.71875</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G61" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>134</v>
+      </c>
+      <c r="B62">
+        <v>8</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E62" s="2">
+        <v>0.71944444444444444</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G62" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>71</v>
+      </c>
+      <c r="B63">
+        <v>8</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0.71944444444444444</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G63" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>73</v>
+      </c>
+      <c r="B64">
+        <v>8</v>
+      </c>
+      <c r="C64">
+        <v>2</v>
+      </c>
+      <c r="D64" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0.72013888888888899</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G64" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>45</v>
+      </c>
+      <c r="B65">
+        <v>8</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65" s="1">
+        <v>45134</v>
+      </c>
+      <c r="E65" s="2">
+        <v>0.72013888888888899</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="2"/>
+        <v>0.89668542999999989</v>
+      </c>
+      <c r="G65" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>